<commit_message>
add the extension for chrome and added the javadoc in pom file
</commit_message>
<xml_diff>
--- a/ConfigurationFolder/admin_testcase/TestData.xlsx
+++ b/ConfigurationFolder/admin_testcase/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
   <si>
     <t>End</t>
   </si>
@@ -183,118 +183,163 @@
     <t>TC_EC_0004</t>
   </si>
   <si>
-    <t>register</t>
+    <t>mobilenumber</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>lastname12</t>
+  </si>
+  <si>
+    <t>firstname12</t>
+  </si>
+  <si>
+    <t>gender male/female</t>
+  </si>
+  <si>
+    <t>Birth date</t>
+  </si>
+  <si>
+    <t>Birth month</t>
+  </si>
+  <si>
+    <t>Birth year</t>
+  </si>
+  <si>
+    <t>confirm password</t>
+  </si>
+  <si>
+    <t>display name</t>
+  </si>
+  <si>
+    <t>postal code</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>JAN</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>KW14YT</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>16 Heatherbell Cottages, John O' Groats, Wick, Caithness</t>
+  </si>
+  <si>
+    <t>registrationform</t>
+  </si>
+  <si>
+    <t>registerUsingMobileNumber</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>otp</t>
+  </si>
+  <si>
+    <t>consent_partners</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>consent_cancel</t>
+  </si>
+  <si>
+    <t>accept_consent</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>personaldetail_continue</t>
+  </si>
+  <si>
+    <t>waitForElementInvisible</t>
+  </si>
+  <si>
+    <t>loderclass</t>
+  </si>
+  <si>
+    <t>skip_email</t>
+  </si>
+  <si>
+    <t>competitions</t>
+  </si>
+  <si>
+    <t>TC_EC_0005</t>
+  </si>
+  <si>
+    <t>browsertype</t>
+  </si>
+  <si>
+    <t>SYSTEM_MOBILE_EMULATION</t>
+  </si>
+  <si>
+    <t>navibar</t>
+  </si>
+  <si>
+    <t>1234 560109</t>
+  </si>
+  <si>
+    <t>mobileregisterUsingMobileNumber</t>
+  </si>
+  <si>
+    <t>email11@gmail.com</t>
+  </si>
+  <si>
+    <t>tes11</t>
+  </si>
+  <si>
+    <t>1234 560110</t>
+  </si>
+  <si>
+    <t>email12@gmail.com</t>
+  </si>
+  <si>
+    <t>tes12</t>
+  </si>
+  <si>
+    <t>ture or false ( checked or unchecked)</t>
+  </si>
+  <si>
+    <t>save/ cancel consent</t>
+  </si>
+  <si>
+    <t>cancel</t>
   </si>
   <si>
     <t>entertext</t>
-  </si>
-  <si>
-    <t>mobilenumber</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>continue</t>
-  </si>
-  <si>
-    <t>1234560057</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>enterotp</t>
-  </si>
-  <si>
-    <t>otpcontinue</t>
-  </si>
-  <si>
-    <t>newregistration</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>lastname12</t>
-  </si>
-  <si>
-    <t>firstname12</t>
-  </si>
-  <si>
-    <t>email@gmail.com</t>
-  </si>
-  <si>
-    <t>gender male/female</t>
-  </si>
-  <si>
-    <t>Birth date</t>
-  </si>
-  <si>
-    <t>Birth month</t>
-  </si>
-  <si>
-    <t>Birth year</t>
-  </si>
-  <si>
-    <t>confirm password</t>
-  </si>
-  <si>
-    <t>display name</t>
-  </si>
-  <si>
-    <t>postal code</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>JAN</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>abcd123</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>KW14YT</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>16 Heatherbell Cottages, John O' Groats, Wick, Caithness</t>
   </si>
 </sst>
 </file>
@@ -347,7 +392,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -371,10 +416,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V38"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,7 +772,7 @@
       <c r="C2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -807,7 +853,7 @@
       <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1051,38 +1097,113 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="B28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="D28" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="30">
       <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="B30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="30">
+      <c r="B30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:22">
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>60</v>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31" t="s">
+        <v>100</v>
+      </c>
+      <c r="N31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O31" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -1090,151 +1211,390 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45">
+      <c r="B33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="B52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" ht="30">
+      <c r="B55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" ht="30">
+      <c r="B56" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="B33" s="1" t="s">
+      <c r="F56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L56" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="M56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="B57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E57" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="B34" s="1" t="s">
+      <c r="F57" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57" t="s">
+        <v>74</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I57" t="s">
+        <v>71</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K57" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" t="s">
+        <v>73</v>
+      </c>
+      <c r="M57" t="s">
+        <v>103</v>
+      </c>
+      <c r="N57" t="s">
+        <v>75</v>
+      </c>
+      <c r="O57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:15" ht="30">
-      <c r="B35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M35" s="3" t="s">
+      <c r="C58" t="s">
         <v>82</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="F58" s="11"/>
+      <c r="H58" s="9"/>
+      <c r="J58" s="9"/>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O35" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="B36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" t="s">
-        <v>89</v>
-      </c>
-      <c r="H36" s="10" t="s">
+      <c r="C59" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="H59" s="9"/>
+      <c r="J59" s="9"/>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
         <v>84</v>
       </c>
-      <c r="I36" t="s">
+      <c r="F60" s="11"/>
+      <c r="H60" s="9"/>
+      <c r="J60" s="9"/>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
         <v>85</v>
       </c>
-      <c r="J36" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="F61" s="11"/>
+      <c r="H61" s="9"/>
+      <c r="J61" s="9"/>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" s="11"/>
+      <c r="H62" s="9"/>
+      <c r="J62" s="9"/>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="B63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="L36" t="s">
-        <v>87</v>
-      </c>
-      <c r="M36" t="s">
-        <v>88</v>
-      </c>
-      <c r="N36" t="s">
-        <v>90</v>
-      </c>
-      <c r="O36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" t="s">
+      <c r="F63" s="11"/>
+      <c r="H63" s="9"/>
+      <c r="J63" s="9"/>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="H64" s="9"/>
+      <c r="J64" s="9"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="B65" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" s="11"/>
+      <c r="H65" s="9"/>
+      <c r="J65" s="9"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="F31" r:id="rId2"/>
+    <hyperlink ref="F57" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added the custom Exception and few testcase
</commit_message>
<xml_diff>
--- a/ConfigurationFolder/admin_testcase/TestData.xlsx
+++ b/ConfigurationFolder/admin_testcase/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="152">
   <si>
     <t>End</t>
   </si>
@@ -270,9 +270,6 @@
     <t>consent</t>
   </si>
   <si>
-    <t>consent_cancel</t>
-  </si>
-  <si>
     <t>accept_consent</t>
   </si>
   <si>
@@ -309,27 +306,9 @@
     <t>navibar</t>
   </si>
   <si>
-    <t>1234 560109</t>
-  </si>
-  <si>
     <t>mobileregisterUsingMobileNumber</t>
   </si>
   <si>
-    <t>email11@gmail.com</t>
-  </si>
-  <si>
-    <t>tes11</t>
-  </si>
-  <si>
-    <t>1234 560110</t>
-  </si>
-  <si>
-    <t>email12@gmail.com</t>
-  </si>
-  <si>
-    <t>tes12</t>
-  </si>
-  <si>
     <t>ture or false ( checked or unchecked)</t>
   </si>
   <si>
@@ -339,7 +318,160 @@
     <t>cancel</t>
   </si>
   <si>
-    <t>entertext</t>
+    <t>searchcompetation</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>lodercontainer</t>
+  </si>
+  <si>
+    <t>competition_play</t>
+  </si>
+  <si>
+    <t>competition_applynow_accept</t>
+  </si>
+  <si>
+    <t>competition_applynow_continue</t>
+  </si>
+  <si>
+    <t>mandatoryquestion</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>Yes, Ok</t>
+  </si>
+  <si>
+    <t>Q1Ans</t>
+  </si>
+  <si>
+    <t>Q2Ans</t>
+  </si>
+  <si>
+    <t>Q3Ans</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Treat the Family</t>
+  </si>
+  <si>
+    <t>Q4Ans</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Q5Ans</t>
+  </si>
+  <si>
+    <t>Q6Ans</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Q7Ans</t>
+  </si>
+  <si>
+    <t>Q8Ans</t>
+  </si>
+  <si>
+    <t>Q9Ans</t>
+  </si>
+  <si>
+    <t>Q10Ans</t>
+  </si>
+  <si>
+    <t>competationquestion</t>
+  </si>
+  <si>
+    <t>SingleChoice</t>
+  </si>
+  <si>
+    <t>Boy</t>
+  </si>
+  <si>
+    <t>We all shop for various things. Some of us love shopping and for some of us it is a chore. Today you have to help one of the two characters with your shopping skills. Wear the hat of a shopping expert and here you go... Choose your ROBO character:</t>
+  </si>
+  <si>
+    <t>MultipleChoice</t>
+  </si>
+  <si>
+    <t>Here is the bucket list full of colours. Which colour of apparel would you suggest to ROBO?</t>
+  </si>
+  <si>
+    <t>Bravo! Robo, was wondering if you usually shop alone or with someone? Suggest a good shopping partner to Robo.</t>
+  </si>
+  <si>
+    <t>Do you suggest Robo operates open WiFi while out shopping?</t>
+  </si>
+  <si>
+    <t>Wonderful! Robo loves your selection and finds a true campanion in you. So, Robo wants to know something about you. Robo wants to identify how much you love shopping?</t>
+  </si>
+  <si>
+    <t>Seldom</t>
+  </si>
+  <si>
+    <t>So tell Robo how often you go out shopping?</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Do you regularly play the lottery?</t>
+  </si>
+  <si>
+    <t>Would you like to hear from Your Lotto Service about how you can increase your chances of winning?</t>
+  </si>
+  <si>
+    <t>This question is from Let’s Subscribe, they would like to know if you’d like a free copy of one of the following magazines?</t>
+  </si>
+  <si>
+    <t>Woman's Weekly</t>
+  </si>
+  <si>
+    <t>Can you confirm that you would like to be contacted by Lets Subscribe to arrange your free issue?</t>
+  </si>
+  <si>
+    <t>Pink`Orange`Red`Yellow`Black`Purple`Blue`Green`White</t>
+  </si>
+  <si>
+    <t>Girlfriend/Boyfriend`It is best to shop alone`With Parents`With Friends</t>
+  </si>
+  <si>
+    <t>testing0</t>
+  </si>
+  <si>
+    <t>waitForElementPresent</t>
+  </si>
+  <si>
+    <t>1234560170</t>
+  </si>
+  <si>
+    <t>email60@gmail.com</t>
+  </si>
+  <si>
+    <t>tes60</t>
+  </si>
+  <si>
+    <t>mobile_competitions</t>
+  </si>
+  <si>
+    <t>1234 560185</t>
+  </si>
+  <si>
+    <t>email66@gmail.com</t>
+  </si>
+  <si>
+    <t>tes66</t>
   </si>
 </sst>
 </file>
@@ -724,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,7 +1244,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>80</v>
@@ -1176,7 +1308,7 @@
         <v>61</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="G31" t="s">
         <v>74</v>
@@ -1197,7 +1329,7 @@
         <v>73</v>
       </c>
       <c r="M31" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="N31" t="s">
         <v>75</v>
@@ -1211,379 +1343,883 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45">
-      <c r="B33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>84</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="H32" s="9"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="B42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" t="s">
+        <v>115</v>
+      </c>
+      <c r="H46" t="s">
+        <v>115</v>
+      </c>
+      <c r="I46" t="s">
+        <v>118</v>
+      </c>
+      <c r="J46" t="s">
+        <v>119</v>
+      </c>
+      <c r="K46" t="s">
+        <v>112</v>
+      </c>
+      <c r="L46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="B49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="B50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="B51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="B52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="B53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="B54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="B55" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="B56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="B57" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" t="s">
+        <v>138</v>
+      </c>
+      <c r="E57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="B58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="B62" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="B64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15">
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="2:15">
+      <c r="B66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="2:15">
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="2:15">
+      <c r="B68" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" ht="30">
+      <c r="B69" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" ht="30">
+      <c r="B70" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M70" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O70" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15">
+      <c r="B71" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" t="s">
+        <v>57</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G71" t="s">
+        <v>74</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I71" t="s">
+        <v>71</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K71" t="s">
+        <v>73</v>
+      </c>
+      <c r="L71" t="s">
+        <v>73</v>
+      </c>
+      <c r="M71" t="s">
+        <v>151</v>
+      </c>
+      <c r="N71" t="s">
+        <v>75</v>
+      </c>
+      <c r="O71" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15">
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="F72" s="11"/>
+      <c r="H72" s="9"/>
+      <c r="J72" s="9"/>
+    </row>
+    <row r="73" spans="2:15">
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
         <v>87</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="74" spans="2:15">
+      <c r="B74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15">
+      <c r="B75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15">
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="2:15">
+      <c r="B77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="2:15">
+      <c r="B78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15">
+      <c r="B79" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="2:15">
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="B82" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="B83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12">
+      <c r="B84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="B85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12">
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12">
+      <c r="B89" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C89" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" t="s">
+        <v>108</v>
+      </c>
+      <c r="E89" t="s">
+        <v>112</v>
+      </c>
+      <c r="F89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G89" t="s">
+        <v>115</v>
+      </c>
+      <c r="H89" t="s">
+        <v>115</v>
+      </c>
+      <c r="I89" t="s">
+        <v>118</v>
+      </c>
+      <c r="J89" t="s">
+        <v>119</v>
+      </c>
+      <c r="K89" t="s">
+        <v>112</v>
+      </c>
+      <c r="L89" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12">
+      <c r="B90" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12">
+      <c r="B91" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="B39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="B43" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12">
+      <c r="B92" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" t="s">
+        <v>127</v>
+      </c>
+      <c r="E92" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12">
+      <c r="B93" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C93" t="s">
+        <v>128</v>
+      </c>
+      <c r="D93" t="s">
+        <v>129</v>
+      </c>
+      <c r="E93" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12">
+      <c r="B94" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C94" t="s">
+        <v>128</v>
+      </c>
+      <c r="D94" t="s">
+        <v>130</v>
+      </c>
+      <c r="E94" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12">
+      <c r="B95" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C95" t="s">
+        <v>125</v>
+      </c>
+      <c r="D95" t="s">
+        <v>131</v>
+      </c>
+      <c r="E95" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12">
+      <c r="B96" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C96" t="s">
+        <v>125</v>
+      </c>
+      <c r="D96" t="s">
+        <v>132</v>
+      </c>
+      <c r="E96" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="B97" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" t="s">
+        <v>134</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="B98" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C98" t="s">
+        <v>125</v>
+      </c>
+      <c r="D98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="B99" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C99" t="s">
+        <v>125</v>
+      </c>
+      <c r="D99" t="s">
+        <v>137</v>
+      </c>
+      <c r="E99" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="B100" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100" t="s">
+        <v>125</v>
+      </c>
+      <c r="D100" t="s">
+        <v>138</v>
+      </c>
+      <c r="E100" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="B101" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" t="s">
+        <v>125</v>
+      </c>
+      <c r="D101" t="s">
+        <v>140</v>
+      </c>
+      <c r="E101" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="B48" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15">
-      <c r="B49" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15">
-      <c r="B50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:15">
-      <c r="B51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="2:15">
-      <c r="B52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15">
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15">
-      <c r="B54" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="2:15" ht="30">
-      <c r="B55" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" ht="30">
-      <c r="B56" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M56" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="N56" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="O56" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15">
-      <c r="B57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E57" t="s">
-        <v>61</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G57" t="s">
-        <v>74</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I57" t="s">
-        <v>71</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K57" t="s">
-        <v>73</v>
-      </c>
-      <c r="L57" t="s">
-        <v>73</v>
-      </c>
-      <c r="M57" t="s">
-        <v>103</v>
-      </c>
-      <c r="N57" t="s">
-        <v>75</v>
-      </c>
-      <c r="O57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="2:15">
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>82</v>
-      </c>
-      <c r="F58" s="11"/>
-      <c r="H58" s="9"/>
-      <c r="J58" s="9"/>
-    </row>
-    <row r="59" spans="2:15">
-      <c r="B59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="11"/>
-      <c r="H59" s="9"/>
-      <c r="J59" s="9"/>
-    </row>
-    <row r="60" spans="2:15">
-      <c r="B60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>84</v>
-      </c>
-      <c r="F60" s="11"/>
-      <c r="H60" s="9"/>
-      <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="2:15">
-      <c r="B61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" t="s">
-        <v>85</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="H61" s="9"/>
-      <c r="J61" s="9"/>
-    </row>
-    <row r="62" spans="2:15">
-      <c r="B62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>82</v>
-      </c>
-      <c r="F62" s="11"/>
-      <c r="H62" s="9"/>
-      <c r="J62" s="9"/>
-    </row>
-    <row r="63" spans="2:15">
-      <c r="B63" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="11"/>
-      <c r="H63" s="9"/>
-      <c r="J63" s="9"/>
-    </row>
-    <row r="64" spans="2:15">
-      <c r="B64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>84</v>
-      </c>
-      <c r="F64" s="11"/>
-      <c r="H64" s="9"/>
-      <c r="J64" s="9"/>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="B65" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F65" s="11"/>
-      <c r="H65" s="9"/>
-      <c r="J65" s="9"/>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>56</v>
-      </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" t="s">
+      <c r="B102" s="1"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1591,7 +2227,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="F31" r:id="rId2"/>
-    <hyperlink ref="F57" r:id="rId3"/>
+    <hyperlink ref="F71" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1600,12 +2236,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>